<commit_message>
Atualização automática ADORO PIZZA - 2025-12-09 17:45
</commit_message>
<xml_diff>
--- a/data/custo bebidas.xlsx
+++ b/data/custo bebidas.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvand\Desktop\Adoro Pizza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E4ABA0-9E1B-41B6-8C27-1244733B0427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CDBC65-5C80-4C9E-BB8B-5F7FD940824B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5C2D35E-8C6F-4A5C-84A0-4873509008B8}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{F5C2D35E-8C6F-4A5C-84A0-4873509008B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="ficha tecnica drinks" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="110">
   <si>
     <t>GIN TÔNICA</t>
   </si>
@@ -46,18 +46,9 @@
     <t>MOJITO</t>
   </si>
   <si>
-    <t>MOÇA DE FAMÍLIA</t>
-  </si>
-  <si>
-    <t>MIRANTE DE MINAS</t>
-  </si>
-  <si>
     <t>ROSA MINEIRA</t>
   </si>
   <si>
-    <t>TAÇA IMPORTADO</t>
-  </si>
-  <si>
     <t>COCA COLA 1L</t>
   </si>
   <si>
@@ -253,9 +244,6 @@
     <t>SUCO JARRA</t>
   </si>
   <si>
-    <t>ABACATINHO 2 L</t>
-  </si>
-  <si>
     <t>ABACATINHO 300 ML</t>
   </si>
   <si>
@@ -319,13 +307,58 @@
     <t>fatia no disperdicio</t>
   </si>
   <si>
-    <t>VINHO</t>
-  </si>
-  <si>
     <t>PIZZA FATIA</t>
   </si>
   <si>
     <t>PIZZAS</t>
+  </si>
+  <si>
+    <t>GIN TONICA ESPECIAL</t>
+  </si>
+  <si>
+    <t>ACOMPANHAMENTOS</t>
+  </si>
+  <si>
+    <t>ARROZ BRANCO</t>
+  </si>
+  <si>
+    <t>FAROFA</t>
+  </si>
+  <si>
+    <t>VINAGRETE</t>
+  </si>
+  <si>
+    <t>CACHAÇA CASA AMARELA</t>
+  </si>
+  <si>
+    <t>CACHAÇA MIRANTE DE MINAS ( DOSE )</t>
+  </si>
+  <si>
+    <t>CACHAÇA MOÇA DE FAMÍLIA ( DOSE )</t>
+  </si>
+  <si>
+    <t>CAIPIRINHA DE MARACUJÁ</t>
+  </si>
+  <si>
+    <t>CAIPIVODKA DE MARACUJÁ</t>
+  </si>
+  <si>
+    <t>ABACATINHO 2L</t>
+  </si>
+  <si>
+    <t>TAÇA VINHO IMPORTADO</t>
+  </si>
+  <si>
+    <t>VINHO GARRAFA ( EIQUETA AZUL )</t>
+  </si>
+  <si>
+    <t>VINHO GARRAFA ( ETIQUETA VERDE )</t>
+  </si>
+  <si>
+    <t>VINHO GARRAFA ( ETIQUETA VERMELHA )</t>
+  </si>
+  <si>
+    <t>VINHOS GARRAFA (ETIQUETA AMARELA )</t>
   </si>
 </sst>
 </file>
@@ -362,21 +395,15 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFF0"/>
-        <bgColor rgb="FFF0FFF0"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -399,27 +426,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -432,11 +444,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,11 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB32A3F-7E63-4AF7-B4DC-F4BADFFB9FB2}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,30 +781,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1">
         <v>4</v>
@@ -814,10 +823,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -836,10 +845,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>74</v>
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
       </c>
       <c r="C4" s="1">
         <v>12.9</v>
@@ -858,10 +867,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>75</v>
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
       </c>
       <c r="C5" s="1">
         <v>6.99</v>
@@ -870,20 +879,20 @@
         <v>3.5</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E22" si="0">C5-D5</f>
+        <f>C5-D5</f>
         <v>3.49</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5:F62" si="1">E5/C5</f>
+        <f>E5/C5</f>
         <v>0.49928469241773965</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>76</v>
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
       </c>
       <c r="C6" s="1">
         <v>15</v>
@@ -892,20 +901,20 @@
         <v>4</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f>C6-D6</f>
         <v>11</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" si="1"/>
+        <f>E6/C6</f>
         <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>77</v>
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
       </c>
       <c r="C7" s="1">
         <v>15</v>
@@ -914,784 +923,757 @@
         <v>3</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f>C7-D7</f>
         <v>12</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="1"/>
+        <f>E7/C7</f>
         <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>78</v>
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
       </c>
       <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="1">
+        <f>C8-D8</f>
+        <v>3.5</v>
+      </c>
+      <c r="F8" s="4">
+        <f>E8/C8</f>
         <v>0.5</v>
-      </c>
-      <c r="D8">
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>88</v>
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
+        <f>C9-D9</f>
+        <v>3</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f>E9/C9</f>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>86</v>
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
       </c>
       <c r="C10" s="1">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>C10-D10</f>
+        <v>5</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
+        <f>E10/C10</f>
+        <v>0.38461538461538464</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>85</v>
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
       </c>
       <c r="C11" s="1">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C11-D11</f>
+        <v>18</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="1"/>
-        <v>0.42857142857142855</v>
+        <f>E11/C11</f>
+        <v>0.32727272727272727</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1">
-        <v>48.9</v>
+        <v>7</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <f>30*0.05</f>
+        <v>1.5</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>33.9</v>
+        <f>C12-D12</f>
+        <v>5.5</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.69325153374233128</v>
+        <f>E12/C12</f>
+        <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C13" s="1">
-        <v>0.2</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>0.05</v>
+        <f>30*0.05</f>
+        <v>1.5</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.15000000000000002</v>
+        <f>C13-D13</f>
+        <v>5.5</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="1"/>
-        <v>0.75000000000000011</v>
+        <f>E13/C13</f>
+        <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>81</v>
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
       </c>
       <c r="C14" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>1.5</v>
+        <f>66*0.05</f>
+        <v>3.3000000000000003</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
+        <f>C14-D14</f>
+        <v>3.6999999999999997</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="1"/>
-        <v>0.625</v>
+        <f>E14/C14</f>
+        <v>0.52857142857142858</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="1">
-        <v>5</v>
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
       </c>
       <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1">
+        <f>C16-D16</f>
         <v>3</v>
       </c>
-      <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="F16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f>E16/C16</f>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>79</v>
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
       </c>
       <c r="C17" s="1">
         <v>13</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C17-D17</f>
+        <v>7.5</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="1"/>
-        <v>0.38461538461538464</v>
+        <f>E17/C17</f>
+        <v>0.57692307692307687</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>92</v>
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
       </c>
       <c r="C18" s="1">
-        <v>0.1</v>
+        <v>12</v>
       </c>
       <c r="D18">
-        <v>0.02</v>
+        <v>8.9</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
+        <f>C18-D18</f>
+        <v>3.0999999999999996</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="1"/>
-        <v>0.79999999999999993</v>
+        <f>E18/C18</f>
+        <v>0.2583333333333333</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>93</v>
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
       </c>
       <c r="C19" s="1">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D19">
-        <v>37</v>
+        <v>10.9</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>C19-D19</f>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="1"/>
-        <v>0.32727272727272727</v>
+        <f>E19/C19</f>
+        <v>0.31874999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D20">
-        <v>0.1</v>
+        <v>6</v>
       </c>
       <c r="E20" s="1">
         <f>C20-D20</f>
-        <v>14.9</v>
+        <v>4</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="1"/>
-        <v>0.9933333333333334</v>
+        <f>E20/C20</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>95</v>
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
       </c>
       <c r="C21" s="1">
-        <v>12</v>
+        <v>11.9</v>
       </c>
       <c r="D21">
-        <v>0.1</v>
+        <v>8.9</v>
       </c>
       <c r="E21" s="1">
         <f>C21-D21</f>
-        <v>11.9</v>
+        <v>3</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" si="1"/>
-        <v>0.9916666666666667</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <f>E21/C21</f>
+        <v>0.25210084033613445</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>97</v>
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
       </c>
       <c r="C22" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="0"/>
-        <v>9.5</v>
+        <f>C22-D22</f>
+        <v>4</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="1"/>
-        <v>0.79166666666666663</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <f>E22/C22</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1">
-        <v>0.5</v>
+        <v>15.9</v>
       </c>
       <c r="D23">
-        <v>0.3</v>
+        <f>SUM('ficha tecnica drinks'!E2:E5)</f>
+        <v>4.4950000000000001</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ref="E23:E63" si="2">C23-D23</f>
-        <v>0.2</v>
+        <f>C23-D23</f>
+        <v>11.405000000000001</v>
       </c>
       <c r="F23" s="4">
         <f>E23/C23</f>
-        <v>0.4</v>
+        <v>0.71729559748427674</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1">
-        <v>2</v>
+        <v>15.9</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <f>SUM('ficha tecnica drinks'!E6:E9)</f>
+        <v>5.62</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>C24-D24</f>
+        <v>10.280000000000001</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f>E24/C24</f>
+        <v>0.64654088050314473</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>1.25</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-      <c r="F25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.375</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26">
-        <v>7</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="F26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.42857142857142855</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1">
-        <v>15.9</v>
+        <v>23.9</v>
       </c>
       <c r="D27">
-        <f>SUM('ficha tecnica drinks'!E2:E5)</f>
-        <v>4.4950000000000001</v>
+        <f>SUM('ficha tecnica drinks'!E15:E18)</f>
+        <v>9.27</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="2"/>
-        <v>11.405000000000001</v>
+        <f>C27-D27</f>
+        <v>14.629999999999999</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.71729559748427674</v>
+        <f>E27/C27</f>
+        <v>0.61213389121338913</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="C28" s="1">
-        <v>15.9</v>
+        <v>29.9</v>
       </c>
       <c r="D28">
-        <f>SUM('ficha tecnica drinks'!E6:E9)</f>
-        <v>5.62</v>
+        <f>SUM('ficha tecnica drinks'!E19:E23)</f>
+        <v>13.77</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="2"/>
-        <v>10.280000000000001</v>
+        <f>C28-D28</f>
+        <v>16.13</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.64654088050314473</v>
+        <f>E28/C28</f>
+        <v>0.53946488294314376</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1">
-        <v>3</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D29">
-        <v>2.5</v>
+        <f>SUM('ficha tecnica drinks'!E10:E14)</f>
+        <v>10.474999999999998</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
+        <f>C29-D29</f>
+        <v>6.4250000000000007</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <f>E29/C29</f>
+        <v>0.38017751479289946</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C30" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D30">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="2"/>
-        <v>7.5</v>
+        <f>C30-D30</f>
+        <v>2</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.57692307692307687</v>
+        <f>E30/C30</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1">
-        <v>12</v>
+        <v>0.5</v>
       </c>
       <c r="D31">
-        <v>8.9</v>
+        <v>0.2</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="2"/>
-        <v>3.0999999999999996</v>
+        <f>C31-D31</f>
+        <v>0.3</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2583333333333333</v>
+        <f>E31/C31</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1">
-        <v>16</v>
+        <v>0.2</v>
       </c>
       <c r="D32">
-        <v>10.9</v>
+        <v>0.05</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="2"/>
-        <v>5.0999999999999996</v>
+        <f>C32-D32</f>
+        <v>0.15000000000000002</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.31874999999999998</v>
+        <f>E32/C32</f>
+        <v>0.75000000000000011</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>C33-D33</f>
+        <v>0.5</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f>E33/C33</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="C34" s="1">
-        <v>11.9</v>
+        <v>0.1</v>
       </c>
       <c r="D34">
-        <v>8.9</v>
+        <v>0.02</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f>C34-D34</f>
+        <v>0.08</v>
       </c>
       <c r="F34" s="4">
-        <f t="shared" si="1"/>
-        <v>0.25210084033613445</v>
+        <f>E34/C34</f>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C35" s="1">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="D35">
-        <v>3.5</v>
+        <v>0.3</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
+        <f>C35-D35</f>
+        <v>0.2</v>
       </c>
       <c r="F35" s="4">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
+        <f>E35/C35</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1">
-        <v>10.9</v>
+        <v>2</v>
       </c>
       <c r="D36">
-        <v>6.49</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="2"/>
-        <v>4.41</v>
+        <f>C36-D36</f>
+        <v>1</v>
       </c>
       <c r="F36" s="4">
-        <f t="shared" si="1"/>
-        <v>0.40458715596330275</v>
+        <f>E36/C36</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C37" s="1">
-        <v>16.899999999999999</v>
+        <v>2</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>1.25</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="2"/>
-        <v>6.8999999999999986</v>
+        <f>C37-D37</f>
+        <v>0.75</v>
       </c>
       <c r="F37" s="4">
-        <f t="shared" si="1"/>
-        <v>0.40828402366863903</v>
+        <f>E37/C37</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D38">
-        <v>3.59</v>
+        <v>2.5</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="2"/>
-        <v>3.41</v>
+        <f>C38-D38</f>
+        <v>0.5</v>
       </c>
       <c r="F38" s="4">
-        <f t="shared" si="1"/>
-        <v>0.48714285714285716</v>
+        <f>E38/C38</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C39" s="1">
-        <v>10.9</v>
+        <v>4</v>
       </c>
       <c r="D39">
-        <v>6.49</v>
+        <v>3.5</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="2"/>
-        <v>4.41</v>
+        <f>C39-D39</f>
+        <v>0.5</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="1"/>
-        <v>0.40458715596330275</v>
+        <f>E39/C39</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <v>3.59</v>
+        <v>1.5</v>
       </c>
       <c r="E40" s="1">
-        <f t="shared" si="2"/>
-        <v>3.41</v>
+        <f>C40-D40</f>
+        <v>1.5</v>
       </c>
       <c r="F40" s="4">
-        <f t="shared" si="1"/>
-        <v>0.48714285714285716</v>
+        <f>E40/C40</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C41" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D41">
-        <v>3.59</v>
+        <v>4</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" si="2"/>
-        <v>3.41</v>
+        <f>C41-D41</f>
+        <v>1</v>
       </c>
       <c r="F41" s="4">
-        <f t="shared" si="1"/>
-        <v>0.48714285714285716</v>
+        <f>E41/C41</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C42" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>3.59</v>
+        <v>3.25</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="2"/>
-        <v>3.41</v>
+        <f>C42-D42</f>
+        <v>0.75</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="1"/>
-        <v>0.48714285714285716</v>
+        <f>E42/C42</f>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1699,475 +1681,603 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C43" s="1">
-        <v>23.9</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <f>SUM('ficha tecnica drinks'!E15:E18)</f>
-        <v>9.27</v>
+        <v>2</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="2"/>
-        <v>14.629999999999999</v>
+        <f>C43-D43</f>
+        <v>1</v>
       </c>
       <c r="F43" s="4">
-        <f t="shared" si="1"/>
-        <v>0.61213389121338913</v>
+        <f>E43/C43</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="C44" s="1">
-        <v>29.9</v>
+        <v>4</v>
       </c>
       <c r="D44">
-        <f>SUM('ficha tecnica drinks'!E19:E23)</f>
-        <v>13.77</v>
+        <v>1.5</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="2"/>
-        <v>16.13</v>
+        <f>C44-D44</f>
+        <v>2.5</v>
       </c>
       <c r="F44" s="4">
-        <f t="shared" si="1"/>
-        <v>0.53946488294314376</v>
+        <f>E44/C44</f>
+        <v>0.625</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C45" s="1">
-        <v>9.9</v>
+        <v>12</v>
       </c>
       <c r="D45">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
+        <f>C45-D45</f>
+        <v>9.5</v>
       </c>
       <c r="F45" s="4">
-        <f t="shared" si="1"/>
-        <v>0.44444444444444448</v>
+        <f>E45/C45</f>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="C46" s="1">
-        <v>15.9</v>
+        <v>30</v>
       </c>
       <c r="D46">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="2"/>
-        <v>6.9</v>
+        <f>C46-D46</f>
+        <v>18</v>
       </c>
       <c r="F46" s="4">
-        <f t="shared" si="1"/>
-        <v>0.43396226415094341</v>
+        <f>E46/C46</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B47" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="C47" s="1">
-        <v>7</v>
+        <v>10.9</v>
       </c>
       <c r="D47">
-        <v>2.99</v>
+        <v>6.49</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="2"/>
-        <v>4.01</v>
+        <f>C47-D47</f>
+        <v>4.41</v>
       </c>
       <c r="F47" s="4">
-        <f t="shared" si="1"/>
-        <v>0.57285714285714284</v>
+        <f>E47/C47</f>
+        <v>0.40458715596330275</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C48" s="1">
-        <v>3</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D48">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <f>C48-D48</f>
+        <v>6.8999999999999986</v>
       </c>
       <c r="F48" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f>E48/C48</f>
+        <v>0.40828402366863903</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="C49" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>3.59</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>C49-D49</f>
+        <v>3.41</v>
       </c>
       <c r="F49" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f>E49/C49</f>
+        <v>0.48714285714285716</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="C50" s="1">
-        <v>5</v>
+        <v>10.9</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>6.49</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>C50-D50</f>
+        <v>4.41</v>
       </c>
       <c r="F50" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
+        <f>E50/C50</f>
+        <v>0.40458715596330275</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C51" s="1">
         <v>7</v>
       </c>
       <c r="D51">
-        <f>30*0.05</f>
-        <v>1.5</v>
+        <v>3.59</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" si="2"/>
-        <v>5.5</v>
+        <f>C51-D51</f>
+        <v>3.41</v>
       </c>
       <c r="F51" s="4">
-        <f t="shared" si="1"/>
-        <v>0.7857142857142857</v>
+        <f>E51/C51</f>
+        <v>0.48714285714285716</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C52" s="1">
         <v>7</v>
       </c>
       <c r="D52">
-        <f>30*0.05</f>
-        <v>1.5</v>
+        <v>3.59</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="2"/>
-        <v>5.5</v>
+        <f>C52-D52</f>
+        <v>3.41</v>
       </c>
       <c r="F52" s="4">
-        <f t="shared" si="1"/>
-        <v>0.7857142857142857</v>
+        <f>E52/C52</f>
+        <v>0.48714285714285716</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C53" s="1">
-        <v>16.899999999999999</v>
+        <v>7</v>
       </c>
       <c r="D53">
-        <f>SUM('ficha tecnica drinks'!E10:E14)</f>
-        <v>10.474999999999998</v>
+        <v>3.59</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="2"/>
-        <v>6.4250000000000007</v>
+        <f>C53-D53</f>
+        <v>3.41</v>
       </c>
       <c r="F53" s="4">
-        <f t="shared" si="1"/>
-        <v>0.38017751479289946</v>
+        <f>E53/C53</f>
+        <v>0.48714285714285716</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C54" s="1">
-        <v>7</v>
+        <v>9.9</v>
       </c>
       <c r="D54">
-        <f>66*0.05</f>
-        <v>3.3000000000000003</v>
+        <v>5.5</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="2"/>
-        <v>3.6999999999999997</v>
+        <f>C54-D54</f>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F54" s="4">
-        <f t="shared" si="1"/>
-        <v>0.52857142857142858</v>
+        <f>E54/C54</f>
+        <v>0.44444444444444448</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C55" s="1">
-        <v>7</v>
+        <v>15.9</v>
       </c>
       <c r="D55">
-        <v>3.58</v>
+        <v>9</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="2"/>
-        <v>3.42</v>
+        <f>C55-D55</f>
+        <v>6.9</v>
       </c>
       <c r="F55" s="4">
-        <f t="shared" si="1"/>
-        <v>0.48857142857142855</v>
+        <f>E55/C55</f>
+        <v>0.43396226415094341</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="C56" s="1">
         <v>7</v>
       </c>
       <c r="D56">
-        <v>3.59</v>
+        <v>2.99</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="2"/>
-        <v>3.41</v>
+        <f>C56-D56</f>
+        <v>4.01</v>
       </c>
       <c r="F56" s="4">
-        <f t="shared" si="1"/>
-        <v>0.48714285714285716</v>
+        <f>E56/C56</f>
+        <v>0.57285714285714284</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C57" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57">
-        <v>2.65</v>
+        <v>3.58</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="2"/>
-        <v>5.35</v>
+        <f>C57-D57</f>
+        <v>3.42</v>
       </c>
       <c r="F57" s="4">
-        <f t="shared" si="1"/>
-        <v>0.66874999999999996</v>
+        <f>E57/C57</f>
+        <v>0.48857142857142855</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B58" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="C58" s="1">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D58">
-        <v>5.3</v>
+        <v>3.59</v>
       </c>
       <c r="E58" s="1">
-        <f t="shared" si="2"/>
-        <v>10.7</v>
+        <f>C58-D58</f>
+        <v>3.41</v>
       </c>
       <c r="F58" s="4">
-        <f t="shared" si="1"/>
-        <v>0.66874999999999996</v>
+        <f>E58/C58</f>
+        <v>0.48714285714285716</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C59" s="1">
-        <v>8</v>
+        <v>48.9</v>
       </c>
       <c r="D59">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f>C59-D59</f>
+        <v>33.9</v>
       </c>
       <c r="F59" s="4">
-        <f t="shared" si="1"/>
-        <v>0.375</v>
+        <f>E59/C59</f>
+        <v>0.69325153374233128</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="1">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>0.1</v>
+      </c>
+      <c r="E60" s="1">
+        <f>C60-D60</f>
+        <v>11.9</v>
+      </c>
+      <c r="F60" s="4">
+        <f>E60/C60</f>
+        <v>0.9916666666666667</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="1">
         <v>8</v>
       </c>
-      <c r="C60" s="1">
+      <c r="D61">
+        <v>2.65</v>
+      </c>
+      <c r="E61" s="1">
+        <f>C61-D61</f>
+        <v>5.35</v>
+      </c>
+      <c r="F61" s="4">
+        <f>E61/C61</f>
+        <v>0.66874999999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="1">
+        <v>16</v>
+      </c>
+      <c r="D62">
+        <v>5.3</v>
+      </c>
+      <c r="E62" s="1">
+        <f>C62-D62</f>
+        <v>10.7</v>
+      </c>
+      <c r="F62" s="4">
+        <f>E62/C62</f>
+        <v>0.66874999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="1">
+        <v>8</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63" s="1">
+        <f>C63-D63</f>
+        <v>3</v>
+      </c>
+      <c r="F63" s="4">
+        <f>E63/C63</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" s="1">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>0.1</v>
+      </c>
+      <c r="E64" s="1">
+        <f>C64-D64</f>
+        <v>14.9</v>
+      </c>
+      <c r="F64" s="4">
+        <f>E64/C64</f>
+        <v>0.9933333333333334</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" s="1">
         <v>20</v>
       </c>
-      <c r="D60">
+      <c r="D65">
         <f>45.9*0.3</f>
         <v>13.77</v>
       </c>
-      <c r="E60" s="1">
-        <f t="shared" si="2"/>
+      <c r="E65" s="1">
+        <f>C65-D65</f>
         <v>6.23</v>
       </c>
-      <c r="F60" s="4">
-        <f t="shared" si="1"/>
+      <c r="F65" s="4">
+        <f>E65/C65</f>
         <v>0.3115</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>45</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C61" s="1">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" s="1">
         <v>15</v>
       </c>
-      <c r="D61">
+      <c r="D66">
         <f>25.9*0.3</f>
         <v>7.77</v>
       </c>
-      <c r="E61" s="1">
-        <f t="shared" si="2"/>
+      <c r="E66" s="1">
+        <f>C66-D66</f>
         <v>7.23</v>
       </c>
-      <c r="F61" s="4">
-        <f t="shared" si="1"/>
+      <c r="F66" s="4">
+        <f>E66/C66</f>
         <v>0.48200000000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B62" t="s">
-        <v>60</v>
-      </c>
-      <c r="C62" s="1">
-        <v>4</v>
-      </c>
-      <c r="D62">
-        <v>3.25</v>
-      </c>
-      <c r="E62" s="1">
-        <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-      <c r="F62" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1875</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>46</v>
-      </c>
-      <c r="B63" t="s">
-        <v>61</v>
-      </c>
-      <c r="C63" s="1">
-        <v>3</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
-      </c>
-      <c r="E63" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F63" s="4">
-        <f>E63/C63</f>
-        <v>0.33333333333333331</v>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>95</v>
+      </c>
+      <c r="B67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>95</v>
+      </c>
+      <c r="B69" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C71">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C72">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F63" xr:uid="{ABB32A3F-7E63-4AF7-B4DC-F4BADFFB9FB2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F63">
-      <sortCondition ref="B1:B63"/>
+  <autoFilter ref="A1:F66" xr:uid="{ABB32A3F-7E63-4AF7-B4DC-F4BADFFB9FB2}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
+      <sortCondition ref="A1:A66"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2193,19 +2303,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2213,7 +2323,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3">
         <v>7.4999999999999997E-2</v>
@@ -2231,7 +2341,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
         <v>0.05</v>
@@ -2249,7 +2359,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <v>0.08</v>
@@ -2267,7 +2377,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
         <v>0.3</v>
@@ -2285,7 +2395,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3">
         <v>7.4999999999999997E-2</v>
@@ -2303,7 +2413,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>0.05</v>
@@ -2321,7 +2431,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3">
         <v>0.08</v>
@@ -2339,7 +2449,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>0.3</v>
@@ -2357,7 +2467,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3">
         <v>7.4999999999999997E-2</v>
@@ -2375,7 +2485,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3">
         <v>0.05</v>
@@ -2393,7 +2503,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3">
         <v>0.08</v>
@@ -2411,7 +2521,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -2429,7 +2539,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3">
         <v>0.3</v>
@@ -2447,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3">
         <v>7.4999999999999997E-2</v>
@@ -2465,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -2483,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3">
         <v>0.08</v>
@@ -2501,7 +2611,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3">
         <v>0.3</v>
@@ -2519,7 +2629,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C19" s="3">
         <v>7.4999999999999997E-2</v>
@@ -2537,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3">
         <v>0.05</v>
@@ -2555,7 +2665,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -2573,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3">
         <v>0.08</v>
@@ -2591,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23" s="3">
         <v>0.3</v>

</xml_diff>